<commit_message>
Changes in get price function of the yginance
</commit_message>
<xml_diff>
--- a/230103_Pandas_IBKR.xlsx
+++ b/230103_Pandas_IBKR.xlsx
@@ -1311,16 +1311,16 @@
         <v>22</v>
       </c>
       <c r="G2">
-        <v>137.87</v>
+        <v>143.9600067138672</v>
       </c>
       <c r="H2">
-        <v>3033.14</v>
+        <v>3167.120147705078</v>
       </c>
       <c r="I2">
-        <v>2.53</v>
+        <v>2.57</v>
       </c>
       <c r="J2">
-        <v>3033</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1343,16 +1343,16 @@
         <v>3</v>
       </c>
       <c r="G3">
-        <v>19.35</v>
+        <v>18.65999984741211</v>
       </c>
       <c r="H3">
-        <v>58.05</v>
+        <v>55.97999954223633</v>
       </c>
       <c r="I3">
         <v>0.05</v>
       </c>
       <c r="J3">
-        <v>3091</v>
+        <v>3222</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1375,16 +1375,16 @@
         <v>2</v>
       </c>
       <c r="G4">
-        <v>356.38</v>
+        <v>365.8200073242188</v>
       </c>
       <c r="H4">
-        <v>712.76</v>
+        <v>731.6400146484375</v>
       </c>
       <c r="I4">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="J4">
-        <v>3803</v>
+        <v>3953</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1407,16 +1407,16 @@
         <v>8</v>
       </c>
       <c r="G5">
-        <v>205.9</v>
+        <v>208.4600067138672</v>
       </c>
       <c r="H5">
-        <v>1647.2</v>
+        <v>1667.680053710938</v>
       </c>
       <c r="I5">
-        <v>1.38</v>
+        <v>1.36</v>
       </c>
       <c r="J5">
-        <v>5450</v>
+        <v>5620</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1439,16 +1439,16 @@
         <v>13</v>
       </c>
       <c r="G6">
-        <v>248.49</v>
+        <v>279.4500122070312</v>
       </c>
       <c r="H6">
-        <v>3230.37</v>
+        <v>3632.850158691406</v>
       </c>
       <c r="I6">
-        <v>2.7</v>
+        <v>2.95</v>
       </c>
       <c r="J6">
-        <v>8680</v>
+        <v>9252</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1471,16 +1471,16 @@
         <v>3</v>
       </c>
       <c r="G7">
-        <v>50.98</v>
+        <v>52.84999847412109</v>
       </c>
       <c r="H7">
-        <v>152.94</v>
+        <v>158.5499954223633</v>
       </c>
       <c r="I7">
         <v>0.13</v>
       </c>
       <c r="J7">
-        <v>8832</v>
+        <v>9410</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1503,16 +1503,16 @@
         <v>5</v>
       </c>
       <c r="G8">
-        <v>51.93</v>
+        <v>52.65000152587891</v>
       </c>
       <c r="H8">
-        <v>259.65</v>
+        <v>263.2500076293945</v>
       </c>
       <c r="I8">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="J8">
-        <v>9091</v>
+        <v>9673</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1535,16 +1535,16 @@
         <v>11</v>
       </c>
       <c r="G9">
-        <v>109.65</v>
+        <v>115.5800018310547</v>
       </c>
       <c r="H9">
-        <v>1206.15</v>
+        <v>1271.380020141602</v>
       </c>
       <c r="I9">
-        <v>1.01</v>
+        <v>1.03</v>
       </c>
       <c r="J9">
-        <v>10297</v>
+        <v>10944</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1567,16 +1567,16 @@
         <v>13</v>
       </c>
       <c r="G10">
-        <v>70.06999999999999</v>
+        <v>75.16000366210938</v>
       </c>
       <c r="H10">
-        <v>910.9099999999999</v>
+        <v>977.0800476074219</v>
       </c>
       <c r="I10">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
       <c r="J10">
-        <v>11207</v>
+        <v>11921</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1599,16 +1599,16 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <v>263.24</v>
+        <v>254.8800048828125</v>
       </c>
       <c r="H11">
-        <v>263.24</v>
+        <v>254.8800048828125</v>
       </c>
       <c r="I11">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="J11">
-        <v>11470</v>
+        <v>12175</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1631,16 +1631,16 @@
         <v>21</v>
       </c>
       <c r="G12">
-        <v>97.25</v>
+        <v>99.22000122070312</v>
       </c>
       <c r="H12">
-        <v>2042.25</v>
+        <v>2083.620025634766</v>
       </c>
       <c r="I12">
-        <v>1.71</v>
+        <v>1.69</v>
       </c>
       <c r="J12">
-        <v>13512</v>
+        <v>14258</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1663,16 +1663,16 @@
         <v>4</v>
       </c>
       <c r="G13">
-        <v>4.17</v>
+        <v>4.159999847412109</v>
       </c>
       <c r="H13">
-        <v>16.68</v>
+        <v>16.63999938964844</v>
       </c>
       <c r="I13">
         <v>0.01</v>
       </c>
       <c r="J13">
-        <v>13528</v>
+        <v>14274</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1695,7 +1695,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>2.38</v>
+        <v>2.440000057220459</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1704,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>13528</v>
+        <v>14274</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1727,16 +1727,16 @@
         <v>2</v>
       </c>
       <c r="G15">
-        <v>33.76</v>
+        <v>33.27999877929688</v>
       </c>
       <c r="H15">
-        <v>67.52</v>
+        <v>66.55999755859375</v>
       </c>
       <c r="I15">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="J15">
-        <v>13595</v>
+        <v>14340</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1759,16 +1759,16 @@
         <v>5</v>
       </c>
       <c r="G16">
-        <v>570.78</v>
+        <v>598.5800170898438</v>
       </c>
       <c r="H16">
-        <v>2853.9</v>
+        <v>2992.900085449219</v>
       </c>
       <c r="I16">
-        <v>2.38</v>
+        <v>2.43</v>
       </c>
       <c r="J16">
-        <v>16448</v>
+        <v>17332</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1791,16 +1791,16 @@
         <v>3</v>
       </c>
       <c r="G17">
-        <v>151.6</v>
+        <v>155.8800048828125</v>
       </c>
       <c r="H17">
-        <v>454.8</v>
+        <v>467.6400146484375</v>
       </c>
       <c r="I17">
         <v>0.38</v>
       </c>
       <c r="J17">
-        <v>16902</v>
+        <v>17799</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1823,16 +1823,16 @@
         <v>4</v>
       </c>
       <c r="G18">
-        <v>52.68</v>
+        <v>55.34000015258789</v>
       </c>
       <c r="H18">
-        <v>210.72</v>
+        <v>221.3600006103516</v>
       </c>
       <c r="I18">
         <v>0.18</v>
       </c>
       <c r="J18">
-        <v>17112</v>
+        <v>18020</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1855,16 +1855,16 @@
         <v>5</v>
       </c>
       <c r="G19">
-        <v>4.17</v>
+        <v>4.150000095367432</v>
       </c>
       <c r="H19">
-        <v>20.85</v>
+        <v>20.75000047683716</v>
       </c>
       <c r="I19">
         <v>0.02</v>
       </c>
       <c r="J19">
-        <v>17132</v>
+        <v>18040</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1887,16 +1887,16 @@
         <v>5</v>
       </c>
       <c r="G20">
-        <v>285.77</v>
+        <v>291.9200134277344</v>
       </c>
       <c r="H20">
-        <v>1428.85</v>
+        <v>1459.600067138672</v>
       </c>
       <c r="I20">
         <v>1.19</v>
       </c>
       <c r="J20">
-        <v>18560</v>
+        <v>19499</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1919,16 +1919,16 @@
         <v>3</v>
       </c>
       <c r="G21">
-        <v>6.2</v>
+        <v>6.230000019073486</v>
       </c>
       <c r="H21">
-        <v>18.6</v>
+        <v>18.69000005722046</v>
       </c>
       <c r="I21">
         <v>0.02</v>
       </c>
       <c r="J21">
-        <v>18578</v>
+        <v>19517</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1951,16 +1951,16 @@
         <v>2</v>
       </c>
       <c r="G22">
-        <v>15.12</v>
+        <v>16.19000053405762</v>
       </c>
       <c r="H22">
-        <v>30.24</v>
+        <v>32.38000106811523</v>
       </c>
       <c r="I22">
         <v>0.03</v>
       </c>
       <c r="J22">
-        <v>18608</v>
+        <v>19549</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1983,16 +1983,16 @@
         <v>3</v>
       </c>
       <c r="G23">
-        <v>249.71</v>
+        <v>262.1199951171875</v>
       </c>
       <c r="H23">
-        <v>749.13</v>
+        <v>786.3599853515625</v>
       </c>
       <c r="I23">
-        <v>0.63</v>
+        <v>0.64</v>
       </c>
       <c r="J23">
-        <v>19357</v>
+        <v>20335</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -2015,16 +2015,16 @@
         <v>6</v>
       </c>
       <c r="G24">
-        <v>20.56</v>
+        <v>20.30999946594238</v>
       </c>
       <c r="H24">
-        <v>123.36</v>
+        <v>121.8599967956543</v>
       </c>
       <c r="I24">
         <v>0.1</v>
       </c>
       <c r="J24">
-        <v>19480</v>
+        <v>20456</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2047,16 +2047,16 @@
         <v>3</v>
       </c>
       <c r="G25">
-        <v>396.11</v>
+        <v>410.3900146484375</v>
       </c>
       <c r="H25">
-        <v>1188.33</v>
+        <v>1231.170043945312</v>
       </c>
       <c r="I25">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="J25">
-        <v>20668</v>
+        <v>21687</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -2079,16 +2079,16 @@
         <v>3</v>
       </c>
       <c r="G26">
-        <v>76.15000000000001</v>
+        <v>76.61000061035156</v>
       </c>
       <c r="H26">
-        <v>228.45</v>
+        <v>229.8300018310547</v>
       </c>
       <c r="I26">
         <v>0.19</v>
       </c>
       <c r="J26">
-        <v>20896</v>
+        <v>21916</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2111,16 +2111,16 @@
         <v>10</v>
       </c>
       <c r="G27">
-        <v>23.93</v>
+        <v>22.94000053405762</v>
       </c>
       <c r="H27">
-        <v>239.3</v>
+        <v>229.4000053405762</v>
       </c>
       <c r="I27">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="J27">
-        <v>21135</v>
+        <v>22145</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2143,16 +2143,16 @@
         <v>2</v>
       </c>
       <c r="G28">
-        <v>151.25</v>
+        <v>165.0899963378906</v>
       </c>
       <c r="H28">
-        <v>302.5</v>
+        <v>330.1799926757812</v>
       </c>
       <c r="I28">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="J28">
-        <v>21437</v>
+        <v>22475</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2175,16 +2175,16 @@
         <v>3</v>
       </c>
       <c r="G29">
-        <v>62.42</v>
+        <v>62.58000183105469</v>
       </c>
       <c r="H29">
-        <v>187.26</v>
+        <v>187.7400054931641</v>
       </c>
       <c r="I29">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="J29">
-        <v>21624</v>
+        <v>22662</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2207,16 +2207,16 @@
         <v>31</v>
       </c>
       <c r="G30">
-        <v>39.03</v>
+        <v>39.22000122070312</v>
       </c>
       <c r="H30">
-        <v>1209.93</v>
+        <v>1215.820037841797</v>
       </c>
       <c r="I30">
-        <v>1.01</v>
+        <v>0.99</v>
       </c>
       <c r="J30">
-        <v>22833</v>
+        <v>23877</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2239,16 +2239,16 @@
         <v>10</v>
       </c>
       <c r="G31">
-        <v>9.449999999999999</v>
+        <v>10.13000011444092</v>
       </c>
       <c r="H31">
-        <v>94.5</v>
+        <v>101.3000011444092</v>
       </c>
       <c r="I31">
         <v>0.08</v>
       </c>
       <c r="J31">
-        <v>22927</v>
+        <v>23978</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2271,16 +2271,16 @@
         <v>15</v>
       </c>
       <c r="G32">
-        <v>410.6</v>
+        <v>421.2000122070312</v>
       </c>
       <c r="H32">
-        <v>6159</v>
+        <v>6318.000183105469</v>
       </c>
       <c r="I32">
         <v>5.14</v>
       </c>
       <c r="J32">
-        <v>29086</v>
+        <v>30296</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2303,16 +2303,16 @@
         <v>8</v>
       </c>
       <c r="G33">
-        <v>94.48</v>
+        <v>96.80999755859375</v>
       </c>
       <c r="H33">
-        <v>755.84</v>
+        <v>774.47998046875</v>
       </c>
       <c r="I33">
         <v>0.63</v>
       </c>
       <c r="J33">
-        <v>29841</v>
+        <v>31070</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2335,16 +2335,16 @@
         <v>10</v>
       </c>
       <c r="G34">
-        <v>47.32</v>
+        <v>46.7599983215332</v>
       </c>
       <c r="H34">
-        <v>473.2</v>
+        <v>467.599983215332</v>
       </c>
       <c r="I34">
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
       <c r="J34">
-        <v>30314</v>
+        <v>31537</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2367,16 +2367,16 @@
         <v>2</v>
       </c>
       <c r="G35">
-        <v>125.99</v>
+        <v>129.1399993896484</v>
       </c>
       <c r="H35">
-        <v>251.98</v>
+        <v>258.2799987792969</v>
       </c>
       <c r="I35">
         <v>0.21</v>
       </c>
       <c r="J35">
-        <v>30565</v>
+        <v>31795</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2399,16 +2399,16 @@
         <v>2</v>
       </c>
       <c r="G36">
-        <v>46.66</v>
+        <v>49.15999984741211</v>
       </c>
       <c r="H36">
-        <v>93.31999999999999</v>
+        <v>98.31999969482422</v>
       </c>
       <c r="I36">
         <v>0.08</v>
       </c>
       <c r="J36">
-        <v>30658</v>
+        <v>31893</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2431,16 +2431,16 @@
         <v>8</v>
       </c>
       <c r="G37">
-        <v>8.050000000000001</v>
+        <v>9.069999694824219</v>
       </c>
       <c r="H37">
-        <v>64.40000000000001</v>
+        <v>72.55999755859375</v>
       </c>
       <c r="I37">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="J37">
-        <v>30722</v>
+        <v>31965</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2463,16 +2463,16 @@
         <v>2</v>
       </c>
       <c r="G38">
-        <v>131.82</v>
+        <v>134.5399932861328</v>
       </c>
       <c r="H38">
-        <v>263.64</v>
+        <v>269.0799865722656</v>
       </c>
       <c r="I38">
         <v>0.22</v>
       </c>
       <c r="J38">
-        <v>30985</v>
+        <v>32234</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2495,16 +2495,16 @@
         <v>16</v>
       </c>
       <c r="G39">
-        <v>61.99</v>
+        <v>62.77000045776367</v>
       </c>
       <c r="H39">
-        <v>991.84</v>
+        <v>1004.320007324219</v>
       </c>
       <c r="I39">
-        <v>0.83</v>
+        <v>0.82</v>
       </c>
       <c r="J39">
-        <v>31976</v>
+        <v>33238</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2527,16 +2527,16 @@
         <v>8</v>
       </c>
       <c r="G40">
-        <v>167.87</v>
+        <v>175.4299926757812</v>
       </c>
       <c r="H40">
-        <v>1342.96</v>
+        <v>1403.43994140625</v>
       </c>
       <c r="I40">
-        <v>1.12</v>
+        <v>1.14</v>
       </c>
       <c r="J40">
-        <v>33318</v>
+        <v>34641</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2559,16 +2559,16 @@
         <v>4</v>
       </c>
       <c r="G41">
-        <v>10.24</v>
+        <v>10.27999973297119</v>
       </c>
       <c r="H41">
-        <v>40.96</v>
+        <v>41.11999893188477</v>
       </c>
       <c r="I41">
         <v>0.03</v>
       </c>
       <c r="J41">
-        <v>33358</v>
+        <v>34682</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2591,16 +2591,16 @@
         <v>2</v>
       </c>
       <c r="G42">
-        <v>232.79</v>
+        <v>228.1100006103516</v>
       </c>
       <c r="H42">
-        <v>465.58</v>
+        <v>456.2200012207031</v>
       </c>
       <c r="I42">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="J42">
-        <v>33823</v>
+        <v>35138</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2623,16 +2623,16 @@
         <v>3</v>
       </c>
       <c r="G43">
-        <v>315</v>
+        <v>313.8099975585938</v>
       </c>
       <c r="H43">
-        <v>945</v>
+        <v>941.4299926757812</v>
       </c>
       <c r="I43">
-        <v>0.79</v>
+        <v>0.77</v>
       </c>
       <c r="J43">
-        <v>34768</v>
+        <v>36079</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2655,16 +2655,16 @@
         <v>20</v>
       </c>
       <c r="G44">
-        <v>79.66</v>
+        <v>82.93000030517578</v>
       </c>
       <c r="H44">
-        <v>1593.2</v>
+        <v>1658.600006103516</v>
       </c>
       <c r="I44">
-        <v>1.33</v>
+        <v>1.35</v>
       </c>
       <c r="J44">
-        <v>36361</v>
+        <v>37737</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2687,16 +2687,16 @@
         <v>3</v>
       </c>
       <c r="G45">
-        <v>202.03</v>
+        <v>209.3500061035156</v>
       </c>
       <c r="H45">
-        <v>606.09</v>
+        <v>628.0500183105469</v>
       </c>
       <c r="I45">
         <v>0.51</v>
       </c>
       <c r="J45">
-        <v>36967</v>
+        <v>38365</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2719,16 +2719,16 @@
         <v>20</v>
       </c>
       <c r="G46">
-        <v>214.52</v>
+        <v>220.0099945068359</v>
       </c>
       <c r="H46">
-        <v>4290.400000000001</v>
+        <v>4400.199890136719</v>
       </c>
       <c r="I46">
         <v>3.58</v>
       </c>
       <c r="J46">
-        <v>41257</v>
+        <v>42765</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2751,16 +2751,16 @@
         <v>12</v>
       </c>
       <c r="G47">
-        <v>108.48</v>
+        <v>108.1900024414062</v>
       </c>
       <c r="H47">
-        <v>1301.76</v>
+        <v>1298.280029296875</v>
       </c>
       <c r="I47">
-        <v>1.09</v>
+        <v>1.06</v>
       </c>
       <c r="J47">
-        <v>42558</v>
+        <v>44063</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2783,16 +2783,16 @@
         <v>3</v>
       </c>
       <c r="G48">
-        <v>488.88</v>
+        <v>487</v>
       </c>
       <c r="H48">
-        <v>1466.64</v>
+        <v>1461</v>
       </c>
       <c r="I48">
-        <v>1.22</v>
+        <v>1.19</v>
       </c>
       <c r="J48">
-        <v>44024</v>
+        <v>45524</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2815,16 +2815,16 @@
         <v>2</v>
       </c>
       <c r="G49">
-        <v>112.36</v>
+        <v>110.620002746582</v>
       </c>
       <c r="H49">
-        <v>224.72</v>
+        <v>221.2400054931641</v>
       </c>
       <c r="I49">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="J49">
-        <v>44248</v>
+        <v>45745</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2847,16 +2847,16 @@
         <v>6</v>
       </c>
       <c r="G50">
-        <v>29.22</v>
+        <v>30.09000015258789</v>
       </c>
       <c r="H50">
-        <v>175.32</v>
+        <v>180.5400009155273</v>
       </c>
       <c r="I50">
         <v>0.15</v>
       </c>
       <c r="J50">
-        <v>44423</v>
+        <v>45925</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2879,16 +2879,16 @@
         <v>2</v>
       </c>
       <c r="G51">
-        <v>398.07</v>
+        <v>412.5499877929688</v>
       </c>
       <c r="H51">
-        <v>796.14</v>
+        <v>825.0999755859375</v>
       </c>
       <c r="I51">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="J51">
-        <v>45219</v>
+        <v>46750</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2911,16 +2911,16 @@
         <v>29</v>
       </c>
       <c r="G52">
-        <v>60.01</v>
+        <v>59.15999984741211</v>
       </c>
       <c r="H52">
-        <v>1740.29</v>
+        <v>1715.639995574951</v>
       </c>
       <c r="I52">
-        <v>1.45</v>
+        <v>1.39</v>
       </c>
       <c r="J52">
-        <v>46959</v>
+        <v>48465</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2943,16 +2943,16 @@
         <v>9</v>
       </c>
       <c r="G53">
-        <v>256.77</v>
+        <v>250.5500030517578</v>
       </c>
       <c r="H53">
-        <v>2310.93</v>
+        <v>2254.95002746582</v>
       </c>
       <c r="I53">
-        <v>1.93</v>
+        <v>1.83</v>
       </c>
       <c r="J53">
-        <v>49269</v>
+        <v>50719</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2975,16 +2975,16 @@
         <v>7</v>
       </c>
       <c r="G54">
-        <v>168.74</v>
+        <v>168.8899993896484</v>
       </c>
       <c r="H54">
-        <v>1181.18</v>
+        <v>1182.229995727539</v>
       </c>
       <c r="I54">
-        <v>0.99</v>
+        <v>0.96</v>
       </c>
       <c r="J54">
-        <v>50450</v>
+        <v>51901</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -3007,16 +3007,16 @@
         <v>58</v>
       </c>
       <c r="G55">
-        <v>60.08</v>
+        <v>60.81000137329102</v>
       </c>
       <c r="H55">
-        <v>3484.64</v>
+        <v>3526.980079650879</v>
       </c>
       <c r="I55">
-        <v>2.91</v>
+        <v>2.87</v>
       </c>
       <c r="J55">
-        <v>53934</v>
+        <v>55427</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -3039,16 +3039,16 @@
         <v>7</v>
       </c>
       <c r="G56">
-        <v>44.45</v>
+        <v>44.45999908447266</v>
       </c>
       <c r="H56">
-        <v>311.15</v>
+        <v>311.2199935913086</v>
       </c>
       <c r="I56">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="J56">
-        <v>54245</v>
+        <v>55738</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -3071,16 +3071,16 @@
         <v>7</v>
       </c>
       <c r="G57">
-        <v>45.01</v>
+        <v>45.15999984741211</v>
       </c>
       <c r="H57">
-        <v>315.07</v>
+        <v>316.1199989318848</v>
       </c>
       <c r="I57">
         <v>0.26</v>
       </c>
       <c r="J57">
-        <v>54560</v>
+        <v>56054</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -3103,16 +3103,16 @@
         <v>1</v>
       </c>
       <c r="G58">
-        <v>346.07</v>
+        <v>348.010009765625</v>
       </c>
       <c r="H58">
-        <v>346.07</v>
+        <v>348.010009765625</v>
       </c>
       <c r="I58">
-        <v>0.29</v>
+        <v>0.28</v>
       </c>
       <c r="J58">
-        <v>54906</v>
+        <v>56402</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -3135,16 +3135,16 @@
         <v>3</v>
       </c>
       <c r="G59">
-        <v>443.28</v>
+        <v>459.8099975585938</v>
       </c>
       <c r="H59">
-        <v>1329.84</v>
+        <v>1379.429992675781</v>
       </c>
       <c r="I59">
-        <v>1.11</v>
+        <v>1.12</v>
       </c>
       <c r="J59">
-        <v>56235</v>
+        <v>57781</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -3167,16 +3167,16 @@
         <v>6</v>
       </c>
       <c r="G60">
-        <v>204.53</v>
+        <v>201.8099975585938</v>
       </c>
       <c r="H60">
-        <v>1227.18</v>
+        <v>1210.859985351562</v>
       </c>
       <c r="I60">
-        <v>1.02</v>
+        <v>0.98</v>
       </c>
       <c r="J60">
-        <v>57462</v>
+        <v>58991</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -3199,16 +3199,16 @@
         <v>3</v>
       </c>
       <c r="G61">
-        <v>11.26</v>
+        <v>12.22000026702881</v>
       </c>
       <c r="H61">
-        <v>33.78</v>
+        <v>36.66000080108643</v>
       </c>
       <c r="I61">
         <v>0.03</v>
       </c>
       <c r="J61">
-        <v>57495</v>
+        <v>59027</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -3231,16 +3231,16 @@
         <v>4</v>
       </c>
       <c r="G62">
-        <v>376.28</v>
+        <v>377.239990234375</v>
       </c>
       <c r="H62">
-        <v>1505.12</v>
+        <v>1508.9599609375</v>
       </c>
       <c r="I62">
-        <v>1.26</v>
+        <v>1.23</v>
       </c>
       <c r="J62">
-        <v>59000</v>
+        <v>60535</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -3263,16 +3263,16 @@
         <v>22</v>
       </c>
       <c r="G63">
-        <v>166.91</v>
+        <v>174.5800018310547</v>
       </c>
       <c r="H63">
-        <v>3672.02</v>
+        <v>3840.760040283203</v>
       </c>
       <c r="I63">
-        <v>3.07</v>
+        <v>3.12</v>
       </c>
       <c r="J63">
-        <v>62672</v>
+        <v>64375</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -3295,16 +3295,16 @@
         <v>3</v>
       </c>
       <c r="G64">
-        <v>50.14</v>
+        <v>50.58000183105469</v>
       </c>
       <c r="H64">
-        <v>150.42</v>
+        <v>151.7400054931641</v>
       </c>
       <c r="I64">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="J64">
-        <v>62822</v>
+        <v>64526</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -3327,16 +3327,16 @@
         <v>3</v>
       </c>
       <c r="G65">
-        <v>100</v>
+        <v>103.9100036621094</v>
       </c>
       <c r="H65">
-        <v>300</v>
+        <v>311.7300109863281</v>
       </c>
       <c r="I65">
         <v>0.25</v>
       </c>
       <c r="J65">
-        <v>63122</v>
+        <v>64837</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -3359,16 +3359,16 @@
         <v>3</v>
       </c>
       <c r="G66">
-        <v>240.22</v>
+        <v>248</v>
       </c>
       <c r="H66">
-        <v>720.66</v>
+        <v>744</v>
       </c>
       <c r="I66">
         <v>0.6</v>
       </c>
       <c r="J66">
-        <v>63842</v>
+        <v>65581</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -3391,16 +3391,16 @@
         <v>28</v>
       </c>
       <c r="G67">
-        <v>81.81999999999999</v>
+        <v>76.40000152587891</v>
       </c>
       <c r="H67">
-        <v>2290.96</v>
+        <v>2139.200042724609</v>
       </c>
       <c r="I67">
-        <v>1.91</v>
+        <v>1.74</v>
       </c>
       <c r="J67">
-        <v>66132</v>
+        <v>67720</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -3423,16 +3423,16 @@
         <v>4</v>
       </c>
       <c r="G68">
-        <v>126.62</v>
+        <v>127.5299987792969</v>
       </c>
       <c r="H68">
-        <v>506.48</v>
+        <v>510.1199951171875</v>
       </c>
       <c r="I68">
-        <v>0.42</v>
+        <v>0.41</v>
       </c>
       <c r="J68">
-        <v>66638</v>
+        <v>68230</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -3455,16 +3455,16 @@
         <v>3</v>
       </c>
       <c r="G69">
-        <v>11.07</v>
+        <v>12.17000007629395</v>
       </c>
       <c r="H69">
-        <v>33.21</v>
+        <v>36.51000022888184</v>
       </c>
       <c r="I69">
         <v>0.03</v>
       </c>
       <c r="J69">
-        <v>66671</v>
+        <v>68266</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -3487,16 +3487,16 @@
         <v>4</v>
       </c>
       <c r="G70">
-        <v>441.83</v>
+        <v>463.0700073242188</v>
       </c>
       <c r="H70">
-        <v>1767.32</v>
+        <v>1852.280029296875</v>
       </c>
       <c r="I70">
-        <v>1.48</v>
+        <v>1.51</v>
       </c>
       <c r="J70">
-        <v>68438</v>
+        <v>70118</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -3519,16 +3519,16 @@
         <v>3</v>
       </c>
       <c r="G71">
-        <v>33.85</v>
+        <v>38.63000106811523</v>
       </c>
       <c r="H71">
-        <v>101.55</v>
+        <v>115.8900032043457</v>
       </c>
       <c r="I71">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="J71">
-        <v>68539</v>
+        <v>70233</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -3551,16 +3551,16 @@
         <v>28</v>
       </c>
       <c r="G72">
-        <v>153.47</v>
+        <v>169.8200073242188</v>
       </c>
       <c r="H72">
-        <v>4297.16</v>
+        <v>4754.960205078125</v>
       </c>
       <c r="I72">
-        <v>3.59</v>
+        <v>3.86</v>
       </c>
       <c r="J72">
-        <v>72836</v>
+        <v>74987</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -3583,16 +3583,16 @@
         <v>12</v>
       </c>
       <c r="G73">
-        <v>178.39</v>
+        <v>198.0200042724609</v>
       </c>
       <c r="H73">
-        <v>2140.68</v>
+        <v>2376.240051269531</v>
       </c>
       <c r="I73">
-        <v>1.79</v>
+        <v>1.93</v>
       </c>
       <c r="J73">
-        <v>74976</v>
+        <v>77363</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -3615,16 +3615,16 @@
         <v>6</v>
       </c>
       <c r="G74">
-        <v>87.25</v>
+        <v>89.83000183105469</v>
       </c>
       <c r="H74">
-        <v>523.5</v>
+        <v>538.9800109863281</v>
       </c>
       <c r="I74">
         <v>0.44</v>
       </c>
       <c r="J74">
-        <v>75499</v>
+        <v>77901</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -3647,16 +3647,16 @@
         <v>2</v>
       </c>
       <c r="G75">
-        <v>169.88</v>
+        <v>170.2200012207031</v>
       </c>
       <c r="H75">
-        <v>339.76</v>
+        <v>340.4400024414062</v>
       </c>
       <c r="I75">
         <v>0.28</v>
       </c>
       <c r="J75">
-        <v>75838</v>
+        <v>78241</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -3679,16 +3679,16 @@
         <v>15</v>
       </c>
       <c r="G76">
-        <v>45.11</v>
+        <v>44.25</v>
       </c>
       <c r="H76">
-        <v>676.65</v>
+        <v>663.75</v>
       </c>
       <c r="I76">
-        <v>0.5600000000000001</v>
+        <v>0.54</v>
       </c>
       <c r="J76">
-        <v>76514</v>
+        <v>78904</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -3711,16 +3711,16 @@
         <v>12</v>
       </c>
       <c r="G77">
-        <v>142.97</v>
+        <v>141.1499938964844</v>
       </c>
       <c r="H77">
-        <v>1715.64</v>
+        <v>1693.799926757812</v>
       </c>
       <c r="I77">
-        <v>1.43</v>
+        <v>1.38</v>
       </c>
       <c r="J77">
-        <v>78229</v>
+        <v>80597</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -3743,16 +3743,16 @@
         <v>5</v>
       </c>
       <c r="G78">
-        <v>101.82</v>
+        <v>104.3199996948242</v>
       </c>
       <c r="H78">
-        <v>509.1</v>
+        <v>521.5999984741211</v>
       </c>
       <c r="I78">
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
       <c r="J78">
-        <v>78738</v>
+        <v>81118</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -3775,16 +3775,16 @@
         <v>1</v>
       </c>
       <c r="G79">
-        <v>28.43</v>
+        <v>28.6200008392334</v>
       </c>
       <c r="H79">
-        <v>28.43</v>
+        <v>28.6200008392334</v>
       </c>
       <c r="I79">
         <v>0.02</v>
       </c>
       <c r="J79">
-        <v>78766</v>
+        <v>81146</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -3807,16 +3807,16 @@
         <v>5</v>
       </c>
       <c r="G80">
-        <v>122.9</v>
+        <v>133.9600067138672</v>
       </c>
       <c r="H80">
-        <v>614.5</v>
+        <v>669.8000335693359</v>
       </c>
       <c r="I80">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="J80">
-        <v>79380</v>
+        <v>81815</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -3839,16 +3839,16 @@
         <v>5</v>
       </c>
       <c r="G81">
-        <v>94.36</v>
+        <v>100.25</v>
       </c>
       <c r="H81">
-        <v>471.8</v>
+        <v>501.25</v>
       </c>
       <c r="I81">
-        <v>0.39</v>
+        <v>0.41</v>
       </c>
       <c r="J81">
-        <v>79851</v>
+        <v>82316</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -3871,16 +3871,16 @@
         <v>14</v>
       </c>
       <c r="G82">
-        <v>105.04</v>
+        <v>108.7600021362305</v>
       </c>
       <c r="H82">
-        <v>1470.56</v>
+        <v>1522.640029907227</v>
       </c>
       <c r="I82">
-        <v>1.23</v>
+        <v>1.24</v>
       </c>
       <c r="J82">
-        <v>81321</v>
+        <v>83838</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -3903,16 +3903,16 @@
         <v>6</v>
       </c>
       <c r="G83">
-        <v>294.73</v>
+        <v>303.3800048828125</v>
       </c>
       <c r="H83">
-        <v>1768.38</v>
+        <v>1820.280029296875</v>
       </c>
       <c r="I83">
         <v>1.48</v>
       </c>
       <c r="J83">
-        <v>83089</v>
+        <v>85658</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -3935,16 +3935,16 @@
         <v>2</v>
       </c>
       <c r="G84">
-        <v>76.16</v>
+        <v>81.19000244140625</v>
       </c>
       <c r="H84">
-        <v>152.32</v>
+        <v>162.3800048828125</v>
       </c>
       <c r="I84">
         <v>0.13</v>
       </c>
       <c r="J84">
-        <v>83241</v>
+        <v>85820</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -3967,16 +3967,16 @@
         <v>15</v>
       </c>
       <c r="G85">
-        <v>1.09</v>
+        <v>0.9599999785423279</v>
       </c>
       <c r="H85">
-        <v>16.35</v>
+        <v>14.39999967813492</v>
       </c>
       <c r="I85">
         <v>0.01</v>
       </c>
       <c r="J85">
-        <v>83257</v>
+        <v>85834</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -3999,16 +3999,16 @@
         <v>2</v>
       </c>
       <c r="G86">
-        <v>130.22</v>
+        <v>124.4700012207031</v>
       </c>
       <c r="H86">
-        <v>260.44</v>
+        <v>248.9400024414062</v>
       </c>
       <c r="I86">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="J86">
-        <v>83517</v>
+        <v>86082</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -4031,16 +4031,16 @@
         <v>2</v>
       </c>
       <c r="G87">
-        <v>70.63</v>
+        <v>69.91999816894531</v>
       </c>
       <c r="H87">
-        <v>141.26</v>
+        <v>139.8399963378906</v>
       </c>
       <c r="I87">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="J87">
-        <v>83658</v>
+        <v>86221</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -4063,16 +4063,16 @@
         <v>29</v>
       </c>
       <c r="G88">
-        <v>64.7</v>
+        <v>65.48999786376953</v>
       </c>
       <c r="H88">
-        <v>1876.3</v>
+        <v>1899.209938049316</v>
       </c>
       <c r="I88">
-        <v>1.57</v>
+        <v>1.54</v>
       </c>
       <c r="J88">
-        <v>85534</v>
+        <v>88120</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -4095,16 +4095,16 @@
         <v>8</v>
       </c>
       <c r="G89">
-        <v>173</v>
+        <v>174.1000061035156</v>
       </c>
       <c r="H89">
-        <v>1384</v>
+        <v>1392.800048828125</v>
       </c>
       <c r="I89">
-        <v>1.16</v>
+        <v>1.13</v>
       </c>
       <c r="J89">
-        <v>86918</v>
+        <v>89512</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -4127,16 +4127,16 @@
         <v>15</v>
       </c>
       <c r="G90">
-        <v>4.31</v>
+        <v>4.309999942779541</v>
       </c>
       <c r="H90">
-        <v>64.64999999999999</v>
+        <v>64.64999914169312</v>
       </c>
       <c r="I90">
         <v>0.05</v>
       </c>
       <c r="J90">
-        <v>86982</v>
+        <v>89576</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -4159,16 +4159,16 @@
         <v>2</v>
       </c>
       <c r="G91">
-        <v>208.66</v>
+        <v>201.4799957275391</v>
       </c>
       <c r="H91">
-        <v>417.32</v>
+        <v>402.9599914550781</v>
       </c>
       <c r="I91">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="J91">
-        <v>87399</v>
+        <v>89978</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -4191,16 +4191,16 @@
         <v>8</v>
       </c>
       <c r="G92">
-        <v>224.31</v>
+        <v>224.7100067138672</v>
       </c>
       <c r="H92">
-        <v>1794.48</v>
+        <v>1797.680053710938</v>
       </c>
       <c r="I92">
-        <v>1.5</v>
+        <v>1.46</v>
       </c>
       <c r="J92">
-        <v>89193</v>
+        <v>91775</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -4223,16 +4223,16 @@
         <v>6</v>
       </c>
       <c r="G93">
-        <v>124.02</v>
+        <v>126.370002746582</v>
       </c>
       <c r="H93">
-        <v>744.12</v>
+        <v>758.2200164794922</v>
       </c>
       <c r="I93">
         <v>0.62</v>
       </c>
       <c r="J93">
-        <v>89937</v>
+        <v>92533</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -4255,16 +4255,16 @@
         <v>7</v>
       </c>
       <c r="G94">
-        <v>309.84</v>
+        <v>321.0199890136719</v>
       </c>
       <c r="H94">
-        <v>2168.88</v>
+        <v>2247.139923095703</v>
       </c>
       <c r="I94">
-        <v>1.81</v>
+        <v>1.83</v>
       </c>
       <c r="J94">
-        <v>92105</v>
+        <v>94780</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -4287,16 +4287,16 @@
         <v>39</v>
       </c>
       <c r="G95">
-        <v>198.76</v>
+        <v>203.1199951171875</v>
       </c>
       <c r="H95">
-        <v>7751.639999999999</v>
+        <v>7921.679809570312</v>
       </c>
       <c r="I95">
-        <v>6.47</v>
+        <v>6.44</v>
       </c>
       <c r="J95">
-        <v>99856</v>
+        <v>102701</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -4319,16 +4319,16 @@
         <v>1</v>
       </c>
       <c r="G96">
-        <v>11.6</v>
+        <v>11.64000034332275</v>
       </c>
       <c r="H96">
-        <v>11.6</v>
+        <v>11.64000034332275</v>
       </c>
       <c r="I96">
         <v>0.01</v>
       </c>
       <c r="J96">
-        <v>99867</v>
+        <v>102712</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -4351,16 +4351,16 @@
         <v>3</v>
       </c>
       <c r="G97">
-        <v>40</v>
+        <v>40.27000045776367</v>
       </c>
       <c r="H97">
-        <v>120</v>
+        <v>120.810001373291</v>
       </c>
       <c r="I97">
         <v>0.1</v>
       </c>
       <c r="J97">
-        <v>99987</v>
+        <v>102832</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -4383,16 +4383,16 @@
         <v>3</v>
       </c>
       <c r="G98">
-        <v>128.62</v>
+        <v>130.7400054931641</v>
       </c>
       <c r="H98">
-        <v>385.86</v>
+        <v>392.2200164794922</v>
       </c>
       <c r="I98">
         <v>0.32</v>
       </c>
       <c r="J98">
-        <v>100372</v>
+        <v>103224</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -4415,16 +4415,16 @@
         <v>8</v>
       </c>
       <c r="G99">
-        <v>152.06</v>
+        <v>152.5</v>
       </c>
       <c r="H99">
-        <v>1216.48</v>
+        <v>1220</v>
       </c>
       <c r="I99">
-        <v>1.02</v>
+        <v>0.99</v>
       </c>
       <c r="J99">
-        <v>101588</v>
+        <v>104444</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -4447,16 +4447,16 @@
         <v>10</v>
       </c>
       <c r="G100">
-        <v>140.54</v>
+        <v>142.2100067138672</v>
       </c>
       <c r="H100">
-        <v>1405.4</v>
+        <v>1422.100067138672</v>
       </c>
       <c r="I100">
-        <v>1.17</v>
+        <v>1.16</v>
       </c>
       <c r="J100">
-        <v>102993</v>
+        <v>105866</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -4479,16 +4479,16 @@
         <v>3</v>
       </c>
       <c r="G101">
-        <v>46.54</v>
+        <v>46.93000030517578</v>
       </c>
       <c r="H101">
-        <v>139.62</v>
+        <v>140.7900009155273</v>
       </c>
       <c r="I101">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="J101">
-        <v>103132</v>
+        <v>106006</v>
       </c>
     </row>
     <row r="102" spans="1:10">
@@ -4511,16 +4511,16 @@
         <v>11</v>
       </c>
       <c r="G102">
-        <v>15.41</v>
+        <v>15.30000019073486</v>
       </c>
       <c r="H102">
-        <v>169.51</v>
+        <v>168.3000020980835</v>
       </c>
       <c r="I102">
         <v>0.14</v>
       </c>
       <c r="J102">
-        <v>103301</v>
+        <v>106174</v>
       </c>
     </row>
     <row r="103" spans="1:10">
@@ -4543,16 +4543,16 @@
         <v>5</v>
       </c>
       <c r="G103">
-        <v>110.18</v>
+        <v>101.3300018310547</v>
       </c>
       <c r="H103">
-        <v>550.9000000000001</v>
+        <v>506.6500091552734</v>
       </c>
       <c r="I103">
-        <v>0.46</v>
+        <v>0.41</v>
       </c>
       <c r="J103">
-        <v>103851</v>
+        <v>106680</v>
       </c>
     </row>
     <row r="104" spans="1:10">
@@ -4575,16 +4575,16 @@
         <v>7</v>
       </c>
       <c r="G104">
-        <v>267.56</v>
+        <v>273.2200012207031</v>
       </c>
       <c r="H104">
-        <v>1872.92</v>
+        <v>1912.540008544922</v>
       </c>
       <c r="I104">
-        <v>1.56</v>
+        <v>1.55</v>
       </c>
       <c r="J104">
-        <v>105723</v>
+        <v>108592</v>
       </c>
     </row>
     <row r="105" spans="1:10">
@@ -4607,16 +4607,16 @@
         <v>2</v>
       </c>
       <c r="G105">
-        <v>39.75</v>
+        <v>39.63999938964844</v>
       </c>
       <c r="H105">
-        <v>79.5</v>
+        <v>79.27999877929688</v>
       </c>
       <c r="I105">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="J105">
-        <v>105802</v>
+        <v>108671</v>
       </c>
     </row>
     <row r="106" spans="1:10">
@@ -4639,16 +4639,16 @@
         <v>7</v>
       </c>
       <c r="G106">
-        <v>342.5</v>
+        <v>364.8699951171875</v>
       </c>
       <c r="H106">
-        <v>2397.5</v>
+        <v>2554.089965820312</v>
       </c>
       <c r="I106">
-        <v>2</v>
+        <v>2.08</v>
       </c>
       <c r="J106">
-        <v>108199</v>
+        <v>111225</v>
       </c>
     </row>
     <row r="107" spans="1:10">
@@ -4671,16 +4671,16 @@
         <v>5</v>
       </c>
       <c r="G107">
-        <v>212.07</v>
+        <v>226.7200012207031</v>
       </c>
       <c r="H107">
-        <v>1060.35</v>
+        <v>1133.600006103516</v>
       </c>
       <c r="I107">
-        <v>0.89</v>
+        <v>0.92</v>
       </c>
       <c r="J107">
-        <v>109259</v>
+        <v>112358</v>
       </c>
     </row>
     <row r="108" spans="1:10">
@@ -4703,16 +4703,16 @@
         <v>35</v>
       </c>
       <c r="G108">
-        <v>98.02</v>
+        <v>97.51999664306641</v>
       </c>
       <c r="H108">
-        <v>3430.7</v>
+        <v>3413.199882507324</v>
       </c>
       <c r="I108">
-        <v>2.86</v>
+        <v>2.77</v>
       </c>
       <c r="J108">
-        <v>112689</v>
+        <v>115771</v>
       </c>
     </row>
     <row r="109" spans="1:10">
@@ -4735,16 +4735,16 @@
         <v>6</v>
       </c>
       <c r="G109">
-        <v>472.5</v>
+        <v>497.75</v>
       </c>
       <c r="H109">
-        <v>2835</v>
+        <v>2986.5</v>
       </c>
       <c r="I109">
-        <v>2.37</v>
+        <v>2.43</v>
       </c>
       <c r="J109">
-        <v>115524</v>
+        <v>118757</v>
       </c>
     </row>
     <row r="110" spans="1:10">
@@ -4767,16 +4767,16 @@
         <v>6</v>
       </c>
       <c r="G110">
-        <v>497.3</v>
+        <v>499.3599853515625</v>
       </c>
       <c r="H110">
-        <v>2983.8</v>
+        <v>2996.159912109375</v>
       </c>
       <c r="I110">
-        <v>2.49</v>
+        <v>2.44</v>
       </c>
       <c r="J110">
-        <v>118507</v>
+        <v>121753</v>
       </c>
     </row>
     <row r="111" spans="1:10">
@@ -4799,16 +4799,16 @@
         <v>3</v>
       </c>
       <c r="G111">
-        <v>157.99</v>
+        <v>160.5</v>
       </c>
       <c r="H111">
-        <v>473.97</v>
+        <v>481.5</v>
       </c>
       <c r="I111">
-        <v>0.4</v>
+        <v>0.39</v>
       </c>
       <c r="J111">
-        <v>118980</v>
+        <v>122234</v>
       </c>
     </row>
     <row r="112" spans="1:10">
@@ -4831,16 +4831,16 @@
         <v>3</v>
       </c>
       <c r="G112">
-        <v>67.12</v>
+        <v>67.51999664306641</v>
       </c>
       <c r="H112">
-        <v>201.36</v>
+        <v>202.5599899291992</v>
       </c>
       <c r="I112">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="J112">
-        <v>119181</v>
+        <v>122436</v>
       </c>
     </row>
     <row r="113" spans="1:10">
@@ -4863,16 +4863,16 @@
         <v>5</v>
       </c>
       <c r="G113">
-        <v>107.44</v>
+        <v>108.4700012207031</v>
       </c>
       <c r="H113">
-        <v>537.2</v>
+        <v>542.3500061035156</v>
       </c>
       <c r="I113">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="J113">
-        <v>119718</v>
+        <v>122978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>